<commit_message>
fechando o repositorio com as notas do semestre 2025.1
</commit_message>
<xml_diff>
--- a/notas/notas_ia.xlsx
+++ b/notas/notas_ia.xlsx
@@ -462,7 +462,7 @@
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="14">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
@@ -478,13 +478,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="3" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0">
-      <protection hidden="0" locked="1"/>
-    </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
     <xf fontId="2" fillId="3" borderId="0" numFmtId="164" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="164" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2373,7 +2367,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -2387,19 +2381,19 @@
   </cols>
   <sheetData>
     <row r="1" ht="14.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="9" t="s">
         <v>112</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="1" t="s">
         <v>115</v>
       </c>
       <c r="F1" t="s">
@@ -2420,11 +2414,11 @@
       <c r="D2" s="10">
         <v>10</v>
       </c>
-      <c r="E2" s="15"/>
+      <c r="E2" s="10"/>
       <c r="F2">
         <v>6.5</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2">
         <f>(D2+F2)/2</f>
         <v>8.25</v>
       </c>
@@ -2440,11 +2434,11 @@
       <c r="D3" s="10">
         <v>10</v>
       </c>
-      <c r="E3" s="15"/>
+      <c r="E3" s="10"/>
       <c r="F3">
         <v>6.2999999999999998</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3">
         <f>(D3+F3)/2</f>
         <v>8.1500000000000004</v>
       </c>
@@ -2460,11 +2454,11 @@
       <c r="D4" s="10">
         <v>8</v>
       </c>
-      <c r="E4" s="15"/>
+      <c r="E4" s="10"/>
       <c r="F4">
         <v>8.25</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4">
         <f>(D4+F4)/2</f>
         <v>8.125</v>
       </c>
@@ -2476,17 +2470,16 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
-      <c r="C5"/>
       <c r="D5" s="10">
         <v>8.6999999999999993</v>
       </c>
-      <c r="E5" s="15"/>
+      <c r="E5" s="10"/>
       <c r="F5">
         <v>6.75</v>
       </c>
-      <c r="H5" s="10">
-        <f>(D9+F9)/2</f>
-        <v>6.6500000000000004</v>
+      <c r="H5">
+        <f>(D5+F5)/2</f>
+        <v>7.7249999999999996</v>
       </c>
     </row>
     <row r="6" ht="14.25">
@@ -2496,15 +2489,14 @@
       <c r="B6" t="s">
         <v>13</v>
       </c>
-      <c r="C6"/>
       <c r="D6" s="10">
         <v>7.2000000000000002</v>
       </c>
-      <c r="E6" s="15"/>
+      <c r="E6" s="10"/>
       <c r="F6">
         <v>7.5499999999999998</v>
       </c>
-      <c r="H6" s="10">
+      <c r="H6">
         <f>(D6+F6)/2</f>
         <v>7.375</v>
       </c>
@@ -2520,11 +2512,11 @@
       <c r="D7" s="10">
         <v>8</v>
       </c>
-      <c r="E7" s="15"/>
+      <c r="E7" s="10"/>
       <c r="F7">
         <v>6.3499999999999996</v>
       </c>
-      <c r="H7" s="10">
+      <c r="H7">
         <f>(D7+F7)/2</f>
         <v>7.1749999999999998</v>
       </c>
@@ -2540,13 +2532,13 @@
       <c r="D8" s="10">
         <v>7</v>
       </c>
-      <c r="E8" s="15"/>
+      <c r="E8" s="10"/>
       <c r="F8">
         <v>7.0499999999999998</v>
       </c>
-      <c r="H8" s="10">
-        <f>(D10+F10)/2</f>
-        <v>6.6500000000000004</v>
+      <c r="H8">
+        <f>(D8+F8)/2</f>
+        <v>7.0250000000000004</v>
       </c>
     </row>
     <row r="9" ht="14.25">
@@ -2560,11 +2552,11 @@
       <c r="D9" s="10">
         <v>8</v>
       </c>
-      <c r="E9" s="15"/>
+      <c r="E9" s="10"/>
       <c r="F9">
         <v>5.2999999999999998</v>
       </c>
-      <c r="H9" s="10">
+      <c r="H9">
         <f>(D9+F9)/2</f>
         <v>6.6500000000000004</v>
       </c>
@@ -2576,17 +2568,16 @@
       <c r="B10" t="s">
         <v>13</v>
       </c>
-      <c r="C10"/>
       <c r="D10" s="10">
         <v>6.5</v>
       </c>
-      <c r="E10" s="15"/>
+      <c r="E10" s="10"/>
       <c r="F10">
         <v>6.7999999999999998</v>
       </c>
-      <c r="H10" s="10">
-        <f>(D12+F12)/2</f>
-        <v>6.2750000000000004</v>
+      <c r="H10">
+        <f>(D10+F10)/2</f>
+        <v>6.6500000000000004</v>
       </c>
     </row>
     <row r="11" ht="14.25">
@@ -2600,13 +2591,13 @@
       <c r="D11" s="10">
         <v>4.375</v>
       </c>
-      <c r="E11" s="15"/>
+      <c r="E11" s="10"/>
       <c r="F11">
         <v>8.9000000000000004</v>
       </c>
-      <c r="H11" s="10">
-        <f>(D12+F12)/2</f>
-        <v>6.2750000000000004</v>
+      <c r="H11">
+        <f>(D11+F11)/2</f>
+        <v>6.6375000000000002</v>
       </c>
     </row>
     <row r="12" ht="14.25">
@@ -2620,11 +2611,11 @@
       <c r="D12" s="10">
         <v>8</v>
       </c>
-      <c r="E12" s="15"/>
+      <c r="E12" s="10"/>
       <c r="F12">
         <v>4.5499999999999998</v>
       </c>
-      <c r="H12" s="10">
+      <c r="H12">
         <f>(D12+F12)/2</f>
         <v>6.2750000000000004</v>
       </c>
@@ -2640,11 +2631,11 @@
       <c r="D13" s="10">
         <v>4.375</v>
       </c>
-      <c r="E13" s="15"/>
+      <c r="E13" s="10"/>
       <c r="F13">
         <v>7.9500000000000002</v>
       </c>
-      <c r="H13" s="10">
+      <c r="H13">
         <f>(D13+F13)/2</f>
         <v>6.1624999999999996</v>
       </c>
@@ -2660,13 +2651,13 @@
       <c r="D14" s="10">
         <v>4.375</v>
       </c>
-      <c r="E14" s="15"/>
+      <c r="E14" s="10"/>
       <c r="F14">
         <v>7.7999999999999998</v>
       </c>
-      <c r="H14" s="10">
-        <f>(D15+F15)/2</f>
-        <v>6</v>
+      <c r="H14">
+        <f>(D14+F14)/2</f>
+        <v>6.0875000000000004</v>
       </c>
     </row>
     <row r="15" ht="14.25">
@@ -2680,11 +2671,11 @@
       <c r="D15" s="10">
         <v>3.75</v>
       </c>
-      <c r="E15" s="15"/>
+      <c r="E15" s="10"/>
       <c r="F15">
         <v>8.25</v>
       </c>
-      <c r="H15" s="10">
+      <c r="H15">
         <f>(D15+F15)/2</f>
         <v>6</v>
       </c>
@@ -2696,15 +2687,14 @@
       <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C16"/>
       <c r="D16" s="10">
         <v>4.5</v>
       </c>
-      <c r="E16" s="15"/>
+      <c r="E16" s="10"/>
       <c r="F16">
         <v>7.2999999999999998</v>
       </c>
-      <c r="H16" s="10">
+      <c r="H16">
         <f>(D16+F16)/2</f>
         <v>5.9000000000000004</v>
       </c>
@@ -2720,13 +2710,13 @@
       <c r="D17" s="10">
         <v>5.25</v>
       </c>
-      <c r="E17" s="15"/>
+      <c r="E17" s="10"/>
       <c r="F17">
         <v>6.5</v>
       </c>
-      <c r="H17" s="10">
-        <f>(D19+F19)/2</f>
-        <v>5.4375</v>
+      <c r="H17">
+        <f>(D17+F17)/2</f>
+        <v>5.875</v>
       </c>
     </row>
     <row r="18" ht="14.25">
@@ -2736,15 +2726,14 @@
       <c r="B18" t="s">
         <v>13</v>
       </c>
-      <c r="C18"/>
       <c r="D18" s="10">
         <v>4.75</v>
       </c>
-      <c r="E18" s="15"/>
+      <c r="E18" s="10"/>
       <c r="F18">
         <v>6.9000000000000004</v>
       </c>
-      <c r="H18" s="10">
+      <c r="H18">
         <f>(D18+F18)/2</f>
         <v>5.8250000000000002</v>
       </c>
@@ -2760,11 +2749,11 @@
       <c r="D19" s="10">
         <v>2.875</v>
       </c>
-      <c r="E19" s="15"/>
+      <c r="E19" s="10"/>
       <c r="F19">
         <v>8</v>
       </c>
-      <c r="H19" s="10">
+      <c r="H19">
         <f>(D19+F19)/2</f>
         <v>5.4375</v>
       </c>
@@ -2780,11 +2769,11 @@
       <c r="D20" s="10">
         <v>2.875</v>
       </c>
-      <c r="E20" s="15"/>
+      <c r="E20" s="10"/>
       <c r="F20">
         <v>8</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20">
         <f>(D20+F20)/2</f>
         <v>5.4375</v>
       </c>
@@ -2796,17 +2785,16 @@
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21"/>
       <c r="D21" s="10">
         <v>3.875</v>
       </c>
-      <c r="E21" s="15"/>
+      <c r="E21" s="10"/>
       <c r="F21">
         <v>6.7999999999999998</v>
       </c>
-      <c r="H21" s="10">
-        <f>(D26+F26)/2</f>
-        <v>4.7750000000000004</v>
+      <c r="H21">
+        <f>(D21+F21)/2</f>
+        <v>5.3375000000000004</v>
       </c>
     </row>
     <row r="22" ht="14.25">
@@ -2820,11 +2808,11 @@
       <c r="D22" s="10">
         <v>2.875</v>
       </c>
-      <c r="E22" s="15"/>
+      <c r="E22" s="10"/>
       <c r="F22">
         <v>7.5</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22">
         <f>(D22+F22)/2</f>
         <v>5.1875</v>
       </c>
@@ -2836,17 +2824,16 @@
       <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="C23"/>
       <c r="D23" s="10">
         <v>3.875</v>
       </c>
-      <c r="E23" s="15"/>
+      <c r="E23" s="10"/>
       <c r="F23">
         <v>6.5</v>
       </c>
-      <c r="H23" s="10">
-        <f>(D26+F26)/2</f>
-        <v>4.7750000000000004</v>
+      <c r="H23">
+        <f>(D23+F23)/2</f>
+        <v>5.1875</v>
       </c>
     </row>
     <row r="24" ht="14.25">
@@ -2860,13 +2847,13 @@
       <c r="D24" s="10">
         <v>2.875</v>
       </c>
-      <c r="E24" s="15"/>
+      <c r="E24" s="10"/>
       <c r="F24">
         <v>7.0499999999999998</v>
       </c>
-      <c r="H24" s="10">
-        <f>(D29+F29)/2</f>
-        <v>4.3499999999999996</v>
+      <c r="H24">
+        <f>(D24+F24)/2</f>
+        <v>4.9625000000000004</v>
       </c>
     </row>
     <row r="25" ht="14.25">
@@ -2880,11 +2867,11 @@
       <c r="D25" s="10">
         <v>2.25</v>
       </c>
-      <c r="E25" s="15"/>
+      <c r="E25" s="10"/>
       <c r="F25">
         <v>7.5499999999999998</v>
       </c>
-      <c r="H25" s="10">
+      <c r="H25">
         <f>(D25+F25)/2</f>
         <v>4.9000000000000004</v>
       </c>
@@ -2900,11 +2887,11 @@
       <c r="D26" s="10">
         <v>3.75</v>
       </c>
-      <c r="E26" s="15"/>
+      <c r="E26" s="10"/>
       <c r="F26">
         <v>5.7999999999999998</v>
       </c>
-      <c r="H26" s="10">
+      <c r="H26">
         <f>(D26+F26)/2</f>
         <v>4.7750000000000004</v>
       </c>
@@ -2920,11 +2907,11 @@
       <c r="D27" s="10">
         <v>3.5</v>
       </c>
-      <c r="E27" s="15"/>
+      <c r="E27" s="10"/>
       <c r="F27">
         <v>6</v>
       </c>
-      <c r="H27" s="10">
+      <c r="H27">
         <f>(D27+F27)/2</f>
         <v>4.75</v>
       </c>
@@ -2940,11 +2927,11 @@
       <c r="D28" s="10">
         <v>3.75</v>
       </c>
-      <c r="E28" s="15"/>
+      <c r="E28" s="10"/>
       <c r="F28">
         <v>5.4500000000000002</v>
       </c>
-      <c r="H28" s="10">
+      <c r="H28">
         <f>(D28+F28)/2</f>
         <v>4.5999999999999996</v>
       </c>
@@ -2959,16 +2946,16 @@
       <c r="C29" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="10">
-        <v>0</v>
-      </c>
-      <c r="E29" s="15"/>
+      <c r="D29" s="13">
+        <v>1</v>
+      </c>
+      <c r="E29" s="10"/>
       <c r="F29">
         <v>8.6999999999999993</v>
       </c>
-      <c r="H29" s="16">
+      <c r="H29">
         <f>(D29+F29)/2</f>
-        <v>4.3499999999999996</v>
+        <v>4.8499999999999996</v>
       </c>
     </row>
     <row r="30" ht="14.25">
@@ -2981,16 +2968,16 @@
       <c r="C30" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="10">
-        <v>0</v>
-      </c>
-      <c r="E30" s="15"/>
+      <c r="D30" s="13">
+        <v>1</v>
+      </c>
+      <c r="E30" s="10"/>
       <c r="F30">
         <v>8.4499999999999993</v>
       </c>
-      <c r="H30" s="16">
-        <f>(D32+F32)/2</f>
-        <v>3.6499999999999999</v>
+      <c r="H30">
+        <f>(D30+F30)/2</f>
+        <v>4.7249999999999996</v>
       </c>
     </row>
     <row r="31" ht="14.25">
@@ -3004,13 +2991,13 @@
       <c r="D31" s="10">
         <v>1.375</v>
       </c>
-      <c r="E31" s="15"/>
+      <c r="E31" s="10"/>
       <c r="F31">
         <v>7</v>
       </c>
-      <c r="H31" s="5">
-        <f>(D35+F35)/2</f>
-        <v>2.5</v>
+      <c r="H31">
+        <f>(D31+F31)/2</f>
+        <v>4.1875</v>
       </c>
     </row>
     <row r="32" ht="14.25">
@@ -3024,11 +3011,11 @@
       <c r="D32" s="10">
         <v>0.5</v>
       </c>
-      <c r="E32" s="15"/>
+      <c r="E32" s="10"/>
       <c r="F32">
         <v>6.7999999999999998</v>
       </c>
-      <c r="H32" s="5">
+      <c r="H32">
         <f>(D32+F32)/2</f>
         <v>3.6499999999999999</v>
       </c>
@@ -3043,16 +3030,16 @@
       <c r="C33" t="s">
         <v>22</v>
       </c>
-      <c r="D33" s="10">
-        <v>0</v>
-      </c>
-      <c r="E33" s="15"/>
+      <c r="D33" s="13">
+        <v>4</v>
+      </c>
+      <c r="E33" s="10"/>
       <c r="F33">
         <v>6.5</v>
       </c>
-      <c r="H33" s="16">
+      <c r="H33">
         <f>(D33+F33)/2</f>
-        <v>3.25</v>
+        <v>5.25</v>
       </c>
     </row>
     <row r="34" ht="14.25">
@@ -3065,16 +3052,16 @@
       <c r="C34" t="s">
         <v>22</v>
       </c>
-      <c r="D34" s="10">
-        <v>0</v>
-      </c>
-      <c r="E34" s="15"/>
+      <c r="D34" s="13">
+        <v>3</v>
+      </c>
+      <c r="E34" s="10"/>
       <c r="F34">
         <v>6.5</v>
       </c>
-      <c r="H34" s="16">
+      <c r="H34">
         <f>(D34+F34)/2</f>
-        <v>3.25</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="35" ht="14.25">
@@ -3087,16 +3074,16 @@
       <c r="C35" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="10">
-        <v>0</v>
-      </c>
-      <c r="E35" s="15"/>
+      <c r="D35" s="13">
+        <v>3</v>
+      </c>
+      <c r="E35" s="10"/>
       <c r="F35">
         <v>5</v>
       </c>
-      <c r="H35" s="16">
+      <c r="H35">
         <f>(D35+F35)/2</f>
-        <v>2.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="36" ht="14.25">
@@ -3106,17 +3093,14 @@
       <c r="B36" t="s">
         <v>18</v>
       </c>
-      <c r="C36"/>
       <c r="D36" s="10">
         <v>0</v>
       </c>
-      <c r="E36" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="E36" s="10"/>
       <c r="F36">
         <v>0</v>
       </c>
-      <c r="H36" s="16">
+      <c r="H36">
         <f>(D36+F36)/2</f>
         <v>0</v>
       </c>
@@ -3128,20 +3112,15 @@
       <c r="B37" t="s">
         <v>18</v>
       </c>
-      <c r="C37" t="s">
-        <v>22</v>
-      </c>
       <c r="D37" s="10">
         <v>0</v>
       </c>
-      <c r="E37" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="E37" s="10"/>
       <c r="F37">
         <v>0</v>
       </c>
-      <c r="H37" s="16">
-        <f>(D38+F38)/2</f>
+      <c r="H37">
+        <f>(D37+F37)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -3152,17 +3131,14 @@
       <c r="B38" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C38"/>
       <c r="D38" s="10">
         <v>0</v>
       </c>
-      <c r="E38" s="17" t="s">
-        <v>22</v>
-      </c>
+      <c r="E38" s="10"/>
       <c r="F38">
         <v>0</v>
       </c>
-      <c r="H38" s="16">
+      <c r="H38">
         <f>(D38+F38)/2</f>
         <v>0</v>
       </c>

</xml_diff>